<commit_message>
Meeting documents from Tuesday
</commit_message>
<xml_diff>
--- a/Process-Documents/Meeting-Documents/Meeting Atendance.xlsx
+++ b/Process-Documents/Meeting-Documents/Meeting Atendance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravi_\Documents\GitHub\Treasure-Hunt\Process-Documents\Meeting Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravi_\Documents\GitHub\Treasure-Hunt\Process-Documents\Meeting-Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4CC5EB-4F6C-41E4-ACFF-99D941FDEAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34F64A6-2697-4258-B161-81F07E0EBD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>dates</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>12:30-14:15</t>
+  </si>
+  <si>
+    <t>15:30 - 16:05</t>
   </si>
 </sst>
 </file>
@@ -441,24 +444,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -484,7 +487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43861</v>
       </c>
@@ -498,7 +501,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43864</v>
       </c>
@@ -512,7 +515,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43868</v>
       </c>
@@ -529,7 +532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43872</v>
       </c>
@@ -546,6 +549,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed bugs, added Kanban screenshots and added meeting docs
</commit_message>
<xml_diff>
--- a/Process-Documents/Meeting-Documents/Meeting Atendance.xlsx
+++ b/Process-Documents/Meeting-Documents/Meeting Atendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravi_\Documents\GitHub\Treasure-Hunt\Process-Documents\Meeting-Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60221382-B9DC-4827-9316-483663A93E5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01D8B9C-0224-4FC8-BD4C-6DEB91A3FC93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +634,20 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>43896</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Final Meeting documents :cry:
</commit_message>
<xml_diff>
--- a/Process-Documents/Meeting-Documents/Meeting Atendance.xlsx
+++ b/Process-Documents/Meeting-Documents/Meeting Atendance.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\GitHub\Treasure-Hunt\Process-Documents\Meeting-Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravi_\Documents\GitHub\Treasure-Hunt\Process-Documents\Meeting-Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057A3AC1-A0CD-4AE7-B7A6-608803E9F4CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -460,11 +461,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +656,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>43897</v>
+        <v>43899</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>18</v>

</xml_diff>